<commit_message>
added the new gantt chart and weekly report
</commit_message>
<xml_diff>
--- a/Weekly-Reports/Gantt-Chart.xlsx
+++ b/Weekly-Reports/Gantt-Chart.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="17625" yWindow="5835" windowWidth="19680" windowHeight="11640"/>
+    <workbookView xWindow="17625" yWindow="5835" windowWidth="19440" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="8" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$3:$IQ$29</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Days Remaining</t>
   </si>
@@ -483,9 +483,6 @@
   </si>
   <si>
     <t>Write Report</t>
-  </si>
-  <si>
-    <t>05/14/2012</t>
   </si>
   <si>
     <t>Engr 466 Flim Transport Project</t>
@@ -557,10 +554,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>TBA</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Peripherals Research</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -571,6 +564,12 @@
   <si>
     <t>Initial Design Concepts</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Anderson &amp; Andrew</t>
   </si>
 </sst>
 </file>
@@ -2519,8 +2518,8 @@
   </sheetPr>
   <dimension ref="A1:IQ35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:CH36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2531,7 +2530,7 @@
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" customWidth="1"/>
     <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.7109375" customWidth="1"/>
     <col min="12" max="227" width="0.42578125" customWidth="1"/>
@@ -2557,9 +2556,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:251" ht="14.25">
+    <row r="3" spans="1:251" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:251">
@@ -2589,8 +2588,8 @@
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>20</v>
+      <c r="C8" s="17">
+        <v>41051</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="3" t="s">
@@ -4004,16 +4003,16 @@
       <c r="IP11" s="52"/>
       <c r="IQ11" s="53"/>
     </row>
-    <row r="12" spans="1:251" s="22" customFormat="1" ht="10.5">
+    <row r="12" spans="1:251" s="22" customFormat="1" ht="11.25">
       <c r="A12" s="18"/>
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
       <c r="H12" s="28"/>
     </row>
-    <row r="13" spans="1:251" s="20" customFormat="1" ht="10.5">
+    <row r="13" spans="1:251" s="20" customFormat="1">
       <c r="A13" s="47"/>
       <c r="B13" s="48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="36">
@@ -4021,36 +4020,36 @@
       </c>
       <c r="E13" s="13">
         <f>D13+F13-1</f>
-        <v>41055</v>
+        <v>41061</v>
       </c>
       <c r="F13" s="40">
         <f>MAX(E15:E22)-D13 +1</f>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G13" s="35">
         <f>SUMPRODUCT(F15:F22,G15:G22)/SUM(F15:F22)</f>
-        <v>7.0588235294117658E-3</v>
+        <v>0.21744186046511627</v>
       </c>
       <c r="H13" s="29">
         <f t="shared" ref="H13:H17" si="0">NETWORKDAYS(D13,E13)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I13" s="14">
         <f t="shared" ref="I13:I17" si="1">ROUNDDOWN(G13*F13,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J13" s="29">
         <f>F13-I13</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:251" s="23" customFormat="1" ht="19.5">
+    <row r="14" spans="1:251" s="23" customFormat="1">
       <c r="A14" s="19"/>
       <c r="B14" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="44" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>40</v>
       </c>
       <c r="D14" s="36">
         <v>41043</v>
@@ -4063,7 +4062,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H14" s="30">
         <f t="shared" ref="H14" si="3">NETWORKDAYS(D14,E14)</f>
@@ -4071,11 +4070,11 @@
       </c>
       <c r="I14" s="12">
         <f t="shared" ref="I14" si="4">ROUNDDOWN(G14*F14,0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J14" s="30">
         <f t="shared" ref="J14" si="5">F14-I14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
@@ -4319,13 +4318,13 @@
       <c r="IP14" s="21"/>
       <c r="IQ14" s="21"/>
     </row>
-    <row r="15" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="15" spans="1:251" s="23" customFormat="1">
       <c r="A15" s="19"/>
       <c r="B15" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="36">
         <v>41043</v>
@@ -4594,13 +4593,13 @@
       <c r="IP15" s="21"/>
       <c r="IQ15" s="21"/>
     </row>
-    <row r="16" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="16" spans="1:251" s="23" customFormat="1">
       <c r="A16" s="19"/>
       <c r="B16" s="50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="36">
         <v>41043</v>
@@ -4869,13 +4868,13 @@
       <c r="IP16" s="21"/>
       <c r="IQ16" s="21"/>
     </row>
-    <row r="17" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="17" spans="1:251" s="23" customFormat="1">
       <c r="A17" s="19"/>
       <c r="B17" s="50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="36">
         <v>41043</v>
@@ -4888,7 +4887,7 @@
         <v>10</v>
       </c>
       <c r="G17" s="34">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H17" s="30">
         <f t="shared" si="0"/>
@@ -4896,11 +4895,11 @@
       </c>
       <c r="I17" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J17" s="30">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K17" s="21"/>
       <c r="L17" s="21"/>
@@ -5144,13 +5143,13 @@
       <c r="IP17" s="21"/>
       <c r="IQ17" s="21"/>
     </row>
-    <row r="18" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="18" spans="1:251" s="23" customFormat="1">
       <c r="A18" s="19"/>
       <c r="B18" s="50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D18" s="36">
         <v>41043</v>
@@ -5163,7 +5162,7 @@
         <v>12</v>
       </c>
       <c r="G18" s="34">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="H18" s="30">
         <f>NETWORKDAYS(D18,E18)</f>
@@ -5171,11 +5170,11 @@
       </c>
       <c r="I18" s="12">
         <f>ROUNDDOWN(G18*F18,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J18" s="30">
         <f>F18-I18</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
@@ -5419,13 +5418,13 @@
       <c r="IP18" s="21"/>
       <c r="IQ18" s="21"/>
     </row>
-    <row r="19" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="19" spans="1:251" s="23" customFormat="1">
       <c r="A19" s="49"/>
       <c r="B19" s="50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D19" s="36">
         <v>41045</v>
@@ -5438,7 +5437,7 @@
         <v>10</v>
       </c>
       <c r="G19" s="34">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="H19" s="30">
         <f t="shared" ref="H19:H23" si="13">NETWORKDAYS(D19,E19)</f>
@@ -5446,11 +5445,11 @@
       </c>
       <c r="I19" s="12">
         <f t="shared" ref="I19:I23" si="14">ROUNDDOWN(G19*F19,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J19" s="30">
         <f t="shared" ref="J19:J22" si="15">F19-I19</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
@@ -5694,13 +5693,13 @@
       <c r="IP19" s="21"/>
       <c r="IQ19" s="21"/>
     </row>
-    <row r="20" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="20" spans="1:251" s="23" customFormat="1">
       <c r="A20" s="49"/>
       <c r="B20" s="50" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="36">
         <v>41036</v>
@@ -5713,7 +5712,7 @@
         <v>19</v>
       </c>
       <c r="G20" s="34">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H20" s="30">
         <f t="shared" si="13"/>
@@ -5969,13 +5968,13 @@
       <c r="IP20" s="21"/>
       <c r="IQ20" s="21"/>
     </row>
-    <row r="21" spans="1:251" s="23" customFormat="1" ht="19.5">
+    <row r="21" spans="1:251" s="23" customFormat="1">
       <c r="A21" s="49"/>
       <c r="B21" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="44" t="s">
         <v>45</v>
-      </c>
-      <c r="C21" s="44" t="s">
-        <v>35</v>
       </c>
       <c r="D21" s="36">
         <v>41043</v>
@@ -5988,7 +5987,7 @@
         <v>13</v>
       </c>
       <c r="G21" s="34">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H21" s="30">
         <f t="shared" ref="H21" si="17">NETWORKDAYS(D21,E21)</f>
@@ -5996,11 +5995,11 @@
       </c>
       <c r="I21" s="12">
         <f t="shared" ref="I21" si="18">ROUNDDOWN(G21*F21,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J21" s="30">
         <f t="shared" ref="J21" si="19">F21-I21</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
@@ -6244,30 +6243,30 @@
       <c r="IP21" s="21"/>
       <c r="IQ21" s="21"/>
     </row>
-    <row r="22" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="22" spans="1:251" s="23" customFormat="1">
       <c r="A22" s="49"/>
       <c r="B22" s="50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="36">
-        <v>41049</v>
+        <v>41056</v>
       </c>
       <c r="E22" s="11">
         <f t="shared" si="12"/>
-        <v>41053</v>
+        <v>41061</v>
       </c>
       <c r="F22" s="41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G22" s="34">
         <v>0</v>
       </c>
       <c r="H22" s="30">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="14"/>
@@ -6275,7 +6274,7 @@
       </c>
       <c r="J22" s="30">
         <f t="shared" si="15"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K22" s="21"/>
       <c r="L22" s="21"/>
@@ -6519,10 +6518,10 @@
       <c r="IP22" s="21"/>
       <c r="IQ22" s="21"/>
     </row>
-    <row r="23" spans="1:251" s="20" customFormat="1" ht="10.5">
+    <row r="23" spans="1:251" s="20" customFormat="1">
       <c r="A23" s="47"/>
       <c r="B23" s="48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="43"/>
       <c r="D23" s="36">
@@ -6553,13 +6552,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="24" spans="1:251" s="23" customFormat="1">
       <c r="A24" s="19"/>
       <c r="B24" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="36">
         <v>41054</v>
@@ -6828,13 +6827,13 @@
       <c r="IP24" s="21"/>
       <c r="IQ24" s="21"/>
     </row>
-    <row r="25" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="25" spans="1:251" s="23" customFormat="1">
       <c r="A25" s="19"/>
       <c r="B25" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="36">
         <v>41054</v>
@@ -7103,13 +7102,13 @@
       <c r="IP25" s="21"/>
       <c r="IQ25" s="21"/>
     </row>
-    <row r="26" spans="1:251" s="23" customFormat="1" ht="19.5">
+    <row r="26" spans="1:251" s="23" customFormat="1">
       <c r="A26" s="19"/>
       <c r="B26" s="50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="36">
         <v>41064</v>
@@ -7378,13 +7377,13 @@
       <c r="IP26" s="21"/>
       <c r="IQ26" s="21"/>
     </row>
-    <row r="27" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="27" spans="1:251" s="23" customFormat="1">
       <c r="A27" s="49"/>
       <c r="B27" s="50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D27" s="36">
         <v>41070</v>
@@ -7653,13 +7652,13 @@
       <c r="IP27" s="21"/>
       <c r="IQ27" s="21"/>
     </row>
-    <row r="28" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="28" spans="1:251" s="23" customFormat="1">
       <c r="A28" s="49"/>
       <c r="B28" s="50" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="36">
         <v>41054</v>
@@ -7928,10 +7927,10 @@
       <c r="IP28" s="21"/>
       <c r="IQ28" s="21"/>
     </row>
-    <row r="29" spans="1:251" s="20" customFormat="1" ht="10.5">
+    <row r="29" spans="1:251" s="20" customFormat="1">
       <c r="A29" s="47"/>
       <c r="B29" s="48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="43"/>
       <c r="D29" s="36">
@@ -7962,13 +7961,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="30" spans="1:251" s="23" customFormat="1">
       <c r="A30" s="19"/>
       <c r="B30" s="50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="36">
         <v>41075</v>
@@ -8237,13 +8236,13 @@
       <c r="IP30" s="21"/>
       <c r="IQ30" s="21"/>
     </row>
-    <row r="31" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="31" spans="1:251" s="23" customFormat="1">
       <c r="A31" s="19"/>
       <c r="B31" s="50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="36">
         <v>41094</v>
@@ -8512,13 +8511,13 @@
       <c r="IP31" s="21"/>
       <c r="IQ31" s="21"/>
     </row>
-    <row r="32" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="32" spans="1:251" s="23" customFormat="1">
       <c r="A32" s="49"/>
       <c r="B32" s="50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="36">
         <v>41103</v>
@@ -8787,13 +8786,13 @@
       <c r="IP32" s="21"/>
       <c r="IQ32" s="21"/>
     </row>
-    <row r="33" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="33" spans="1:251" s="23" customFormat="1">
       <c r="A33" s="49"/>
       <c r="B33" s="50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" s="36">
         <v>41110</v>
@@ -9062,10 +9061,10 @@
       <c r="IP33" s="21"/>
       <c r="IQ33" s="21"/>
     </row>
-    <row r="34" spans="1:251" s="20" customFormat="1" ht="10.5">
+    <row r="34" spans="1:251" s="20" customFormat="1">
       <c r="A34" s="47"/>
       <c r="B34" s="48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="43"/>
       <c r="D34" s="36">
@@ -9096,13 +9095,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:251" s="23" customFormat="1" ht="10.5">
+    <row r="35" spans="1:251" s="23" customFormat="1">
       <c r="A35" s="19"/>
       <c r="B35" s="50" t="s">
         <v>19</v>
       </c>
       <c r="C35" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" s="36">
         <v>41117</v>

</xml_diff>

<commit_message>
updated gantt chart and added weekly report 4
</commit_message>
<xml_diff>
--- a/Weekly-Reports/Gantt-Chart.xlsx
+++ b/Weekly-Reports/Gantt-Chart.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="17625" yWindow="5835" windowWidth="19440" windowHeight="11640"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20610" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="8" r:id="rId1"/>
@@ -13,10 +13,10 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$3:$IQ$29</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:ArchID Flags="2"/>
+      <mx:ArchID Flags="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>Days Remaining</t>
   </si>
@@ -570,6 +570,9 @@
   </si>
   <si>
     <t>Anderson &amp; Andrew</t>
+  </si>
+  <si>
+    <t>Andrew</t>
   </si>
 </sst>
 </file>
@@ -2513,13 +2516,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+  <sheetPr published="0" codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IQ35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2556,7 +2559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:251" ht="15.75">
+    <row r="3" spans="1:251" ht="14.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="17">
-        <v>41051</v>
+        <v>41072</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="3" t="s">
@@ -4003,13 +4006,13 @@
       <c r="IP11" s="52"/>
       <c r="IQ11" s="53"/>
     </row>
-    <row r="12" spans="1:251" s="22" customFormat="1" ht="11.25">
+    <row r="12" spans="1:251" s="22" customFormat="1" ht="10.5">
       <c r="A12" s="18"/>
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
       <c r="H12" s="28"/>
     </row>
-    <row r="13" spans="1:251" s="20" customFormat="1">
+    <row r="13" spans="1:251" s="20" customFormat="1" ht="10.5">
       <c r="A13" s="47"/>
       <c r="B13" s="48" t="s">
         <v>21</v>
@@ -4028,7 +4031,7 @@
       </c>
       <c r="G13" s="35">
         <f>SUMPRODUCT(F15:F22,G15:G22)/SUM(F15:F22)</f>
-        <v>0.21744186046511627</v>
+        <v>0.79651162790697672</v>
       </c>
       <c r="H13" s="29">
         <f t="shared" ref="H13:H17" si="0">NETWORKDAYS(D13,E13)</f>
@@ -4036,14 +4039,14 @@
       </c>
       <c r="I13" s="14">
         <f t="shared" ref="I13:I17" si="1">ROUNDDOWN(G13*F13,0)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J13" s="29">
         <f>F13-I13</f>
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:251" s="23" customFormat="1">
+    <row r="14" spans="1:251" s="23" customFormat="1" ht="19.5">
       <c r="A14" s="19"/>
       <c r="B14" s="50" t="s">
         <v>38</v>
@@ -4318,7 +4321,7 @@
       <c r="IP14" s="21"/>
       <c r="IQ14" s="21"/>
     </row>
-    <row r="15" spans="1:251" s="23" customFormat="1">
+    <row r="15" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A15" s="19"/>
       <c r="B15" s="50" t="s">
         <v>41</v>
@@ -4337,7 +4340,7 @@
         <v>6</v>
       </c>
       <c r="G15" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="30">
         <f t="shared" si="0"/>
@@ -4345,11 +4348,11 @@
       </c>
       <c r="I15" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J15" s="30">
         <f t="shared" ref="J15:J17" si="7">F15-I15</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
@@ -4593,7 +4596,7 @@
       <c r="IP15" s="21"/>
       <c r="IQ15" s="21"/>
     </row>
-    <row r="16" spans="1:251" s="23" customFormat="1">
+    <row r="16" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A16" s="19"/>
       <c r="B16" s="50" t="s">
         <v>36</v>
@@ -4612,7 +4615,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="30">
         <f t="shared" ref="H16" si="9">NETWORKDAYS(D16,E16)</f>
@@ -4620,11 +4623,11 @@
       </c>
       <c r="I16" s="12">
         <f t="shared" ref="I16" si="10">ROUNDDOWN(G16*F16,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J16" s="30">
         <f t="shared" ref="J16" si="11">F16-I16</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
@@ -4868,7 +4871,7 @@
       <c r="IP16" s="21"/>
       <c r="IQ16" s="21"/>
     </row>
-    <row r="17" spans="1:251" s="23" customFormat="1">
+    <row r="17" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A17" s="19"/>
       <c r="B17" s="50" t="s">
         <v>35</v>
@@ -5143,7 +5146,7 @@
       <c r="IP17" s="21"/>
       <c r="IQ17" s="21"/>
     </row>
-    <row r="18" spans="1:251" s="23" customFormat="1">
+    <row r="18" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A18" s="19"/>
       <c r="B18" s="50" t="s">
         <v>22</v>
@@ -5418,7 +5421,7 @@
       <c r="IP18" s="21"/>
       <c r="IQ18" s="21"/>
     </row>
-    <row r="19" spans="1:251" s="23" customFormat="1">
+    <row r="19" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A19" s="49"/>
       <c r="B19" s="50" t="s">
         <v>23</v>
@@ -5693,7 +5696,7 @@
       <c r="IP19" s="21"/>
       <c r="IQ19" s="21"/>
     </row>
-    <row r="20" spans="1:251" s="23" customFormat="1">
+    <row r="20" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A20" s="49"/>
       <c r="B20" s="50" t="s">
         <v>19</v>
@@ -5712,7 +5715,7 @@
         <v>19</v>
       </c>
       <c r="G20" s="34">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H20" s="30">
         <f t="shared" si="13"/>
@@ -5720,11 +5723,11 @@
       </c>
       <c r="I20" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J20" s="30">
         <f t="shared" si="15"/>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="K20" s="21"/>
       <c r="L20" s="21"/>
@@ -5968,7 +5971,7 @@
       <c r="IP20" s="21"/>
       <c r="IQ20" s="21"/>
     </row>
-    <row r="21" spans="1:251" s="23" customFormat="1">
+    <row r="21" spans="1:251" s="23" customFormat="1" ht="12" customHeight="1">
       <c r="A21" s="49"/>
       <c r="B21" s="50" t="s">
         <v>43</v>
@@ -5987,7 +5990,7 @@
         <v>13</v>
       </c>
       <c r="G21" s="34">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H21" s="30">
         <f t="shared" ref="H21" si="17">NETWORKDAYS(D21,E21)</f>
@@ -5995,11 +5998,11 @@
       </c>
       <c r="I21" s="12">
         <f t="shared" ref="I21" si="18">ROUNDDOWN(G21*F21,0)</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J21" s="30">
         <f t="shared" ref="J21" si="19">F21-I21</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
@@ -6243,7 +6246,7 @@
       <c r="IP21" s="21"/>
       <c r="IQ21" s="21"/>
     </row>
-    <row r="22" spans="1:251" s="23" customFormat="1">
+    <row r="22" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A22" s="49"/>
       <c r="B22" s="50" t="s">
         <v>37</v>
@@ -6262,7 +6265,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="30">
         <f t="shared" si="13"/>
@@ -6270,11 +6273,11 @@
       </c>
       <c r="I22" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J22" s="30">
         <f t="shared" si="15"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K22" s="21"/>
       <c r="L22" s="21"/>
@@ -6518,7 +6521,7 @@
       <c r="IP22" s="21"/>
       <c r="IQ22" s="21"/>
     </row>
-    <row r="23" spans="1:251" s="20" customFormat="1">
+    <row r="23" spans="1:251" s="20" customFormat="1" ht="10.5">
       <c r="A23" s="47"/>
       <c r="B23" s="48" t="s">
         <v>24</v>
@@ -6537,7 +6540,7 @@
       </c>
       <c r="G23" s="35">
         <f>SUMPRODUCT(F24:F28,G24:G28)/SUM(F24:F28)</f>
-        <v>0</v>
+        <v>0.30462962962962964</v>
       </c>
       <c r="H23" s="29">
         <f t="shared" si="13"/>
@@ -6545,20 +6548,20 @@
       </c>
       <c r="I23" s="14">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J23" s="29">
         <f>F23-I23</f>
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:251" s="23" customFormat="1">
+    <row r="24" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A24" s="19"/>
       <c r="B24" s="50" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D24" s="36">
         <v>41054</v>
@@ -6571,7 +6574,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="34">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="H24" s="30">
         <f>NETWORKDAYS(D24,E24)</f>
@@ -6827,13 +6830,13 @@
       <c r="IP24" s="21"/>
       <c r="IQ24" s="21"/>
     </row>
-    <row r="25" spans="1:251" s="23" customFormat="1">
+    <row r="25" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A25" s="19"/>
       <c r="B25" s="50" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D25" s="36">
         <v>41054</v>
@@ -6846,7 +6849,7 @@
         <v>25</v>
       </c>
       <c r="G25" s="34">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H25" s="30">
         <f>NETWORKDAYS(D25,E25)</f>
@@ -6854,11 +6857,11 @@
       </c>
       <c r="I25" s="12">
         <f>ROUNDDOWN(G25*F25,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J25" s="30">
         <f>F25-I25</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K25" s="21"/>
       <c r="L25" s="21"/>
@@ -7102,13 +7105,13 @@
       <c r="IP25" s="21"/>
       <c r="IQ25" s="21"/>
     </row>
-    <row r="26" spans="1:251" s="23" customFormat="1">
+    <row r="26" spans="1:251" s="23" customFormat="1" ht="12.75" customHeight="1">
       <c r="A26" s="19"/>
       <c r="B26" s="50" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D26" s="36">
         <v>41064</v>
@@ -7121,7 +7124,7 @@
         <v>26</v>
       </c>
       <c r="G26" s="34">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="H26" s="30">
         <f t="shared" ref="H26" si="21">NETWORKDAYS(D26,E26)</f>
@@ -7129,11 +7132,11 @@
       </c>
       <c r="I26" s="12">
         <f t="shared" ref="I26" si="22">ROUNDDOWN(G26*F26,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J26" s="30">
         <f t="shared" ref="J26" si="23">F26-I26</f>
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="K26" s="21"/>
       <c r="L26" s="21"/>
@@ -7377,13 +7380,13 @@
       <c r="IP26" s="21"/>
       <c r="IQ26" s="21"/>
     </row>
-    <row r="27" spans="1:251" s="23" customFormat="1">
+    <row r="27" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A27" s="49"/>
       <c r="B27" s="50" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D27" s="36">
         <v>41070</v>
@@ -7396,7 +7399,7 @@
         <v>20</v>
       </c>
       <c r="G27" s="34">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H27" s="30">
         <f t="shared" ref="H27" si="24">NETWORKDAYS(D27,E27)</f>
@@ -7404,11 +7407,11 @@
       </c>
       <c r="I27" s="12">
         <f t="shared" ref="I27" si="25">ROUNDDOWN(G27*F27,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J27" s="30">
         <f>F27-I27</f>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="K27" s="21"/>
       <c r="L27" s="21"/>
@@ -7652,13 +7655,13 @@
       <c r="IP27" s="21"/>
       <c r="IQ27" s="21"/>
     </row>
-    <row r="28" spans="1:251" s="23" customFormat="1">
+    <row r="28" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A28" s="49"/>
       <c r="B28" s="50" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D28" s="36">
         <v>41054</v>
@@ -7671,7 +7674,7 @@
         <v>36</v>
       </c>
       <c r="G28" s="34">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H28" s="30">
         <f>NETWORKDAYS(D28,E28)</f>
@@ -7679,11 +7682,11 @@
       </c>
       <c r="I28" s="12">
         <f>ROUNDDOWN(G28*F28,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J28" s="30">
         <f>F28-I28</f>
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
@@ -7927,14 +7930,14 @@
       <c r="IP28" s="21"/>
       <c r="IQ28" s="21"/>
     </row>
-    <row r="29" spans="1:251" s="20" customFormat="1">
+    <row r="29" spans="1:251" s="20" customFormat="1" ht="10.5">
       <c r="A29" s="47"/>
       <c r="B29" s="48" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="43"/>
       <c r="D29" s="36">
-        <v>41075</v>
+        <v>41068</v>
       </c>
       <c r="E29" s="13">
         <f>D29+F29-1</f>
@@ -7942,7 +7945,7 @@
       </c>
       <c r="F29" s="40">
         <f>MAX(E30:E33)-D29 +1</f>
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G29" s="35">
         <f>SUMPRODUCT(F30:F33,G30:G33)/SUM(F30:F33)</f>
@@ -7950,7 +7953,7 @@
       </c>
       <c r="H29" s="29">
         <f>NETWORKDAYS(D29,E29)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="I29" s="14">
         <f>ROUNDDOWN(G29*F29,0)</f>
@@ -7958,10 +7961,10 @@
       </c>
       <c r="J29" s="29">
         <f>F29-I29</f>
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:251" s="23" customFormat="1">
+    <row r="30" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A30" s="19"/>
       <c r="B30" s="50" t="s">
         <v>30</v>
@@ -7970,21 +7973,21 @@
         <v>34</v>
       </c>
       <c r="D30" s="36">
-        <v>41075</v>
+        <v>41069</v>
       </c>
       <c r="E30" s="11">
         <f t="shared" ref="E30:E33" si="26">D30+F30-1</f>
-        <v>41094</v>
+        <v>41084</v>
       </c>
       <c r="F30" s="41">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G30" s="34">
         <v>0</v>
       </c>
       <c r="H30" s="30">
         <f>NETWORKDAYS(D30,E30)</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I30" s="12">
         <f>ROUNDDOWN(G30*F30,0)</f>
@@ -7992,7 +7995,7 @@
       </c>
       <c r="J30" s="30">
         <f t="shared" ref="J30:J33" si="27">F30-I30</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K30" s="21"/>
       <c r="L30" s="21"/>
@@ -8236,7 +8239,7 @@
       <c r="IP30" s="21"/>
       <c r="IQ30" s="21"/>
     </row>
-    <row r="31" spans="1:251" s="23" customFormat="1">
+    <row r="31" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A31" s="19"/>
       <c r="B31" s="50" t="s">
         <v>31</v>
@@ -8511,7 +8514,7 @@
       <c r="IP31" s="21"/>
       <c r="IQ31" s="21"/>
     </row>
-    <row r="32" spans="1:251" s="23" customFormat="1">
+    <row r="32" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A32" s="49"/>
       <c r="B32" s="50" t="s">
         <v>32</v>
@@ -8786,7 +8789,7 @@
       <c r="IP32" s="21"/>
       <c r="IQ32" s="21"/>
     </row>
-    <row r="33" spans="1:251" s="23" customFormat="1">
+    <row r="33" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A33" s="49"/>
       <c r="B33" s="50" t="s">
         <v>42</v>
@@ -9061,7 +9064,7 @@
       <c r="IP33" s="21"/>
       <c r="IQ33" s="21"/>
     </row>
-    <row r="34" spans="1:251" s="20" customFormat="1">
+    <row r="34" spans="1:251" s="20" customFormat="1" ht="10.5">
       <c r="A34" s="47"/>
       <c r="B34" s="48" t="s">
         <v>33</v>
@@ -9095,7 +9098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:251" s="23" customFormat="1">
+    <row r="35" spans="1:251" s="23" customFormat="1" ht="10.5">
       <c r="A35" s="19"/>
       <c r="B35" s="50" t="s">
         <v>19</v>
@@ -9449,10 +9452,10 @@
     <hyperlink ref="A1" r:id="rId2" tooltip="Link to Vertex42.com"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="75" orientation="landscape" r:id="rId3"/>
+  <pageSetup scale="75" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -9463,6 +9466,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Update after 2nd report
</commit_message>
<xml_diff>
--- a/Weekly-Reports/Gantt-Chart.xlsx
+++ b/Weekly-Reports/Gantt-Chart.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="19440" windowHeight="15600"/>
+    <workbookView xWindow="-24" yWindow="-24" windowWidth="16608" windowHeight="9432"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="8" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>Days Remaining</t>
   </si>
@@ -570,6 +570,9 @@
   </si>
   <si>
     <t>Anderson &amp; Andrew</t>
+  </si>
+  <si>
+    <t>Andrew</t>
   </si>
 </sst>
 </file>
@@ -2508,33 +2511,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr published="0" codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IQ35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:CC35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DR37" sqref="DR37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.5" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.6640625" customWidth="1"/>
-    <col min="12" max="227" width="0.5" customWidth="1"/>
-    <col min="228" max="251" width="0.5" style="7" customWidth="1"/>
-    <col min="252" max="16384" width="9.1640625" style="7"/>
+    <col min="12" max="227" width="0.44140625" customWidth="1"/>
+    <col min="228" max="251" width="0.44140625" style="7" customWidth="1"/>
+    <col min="252" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:251" customFormat="1" ht="18">
+    <row r="1" spans="1:251" customFormat="1" ht="17.399999999999999">
       <c r="A1" s="39" t="s">
         <v>15</v>
       </c>
@@ -2552,7 +2555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:251" ht="15">
+    <row r="3" spans="1:251" ht="15.6">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2585,7 +2588,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="17">
-        <v>41086</v>
+        <v>41093</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="3" t="s">
@@ -3999,13 +4002,13 @@
       <c r="IP11" s="52"/>
       <c r="IQ11" s="53"/>
     </row>
-    <row r="12" spans="1:251" s="22" customFormat="1" ht="10">
+    <row r="12" spans="1:251" s="22" customFormat="1" ht="10.199999999999999">
       <c r="A12" s="18"/>
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
       <c r="H12" s="28"/>
     </row>
-    <row r="13" spans="1:251" s="20" customFormat="1" ht="10">
+    <row r="13" spans="1:251" s="20" customFormat="1" ht="10.199999999999999">
       <c r="A13" s="47"/>
       <c r="B13" s="48" t="s">
         <v>21</v>
@@ -4024,7 +4027,7 @@
       </c>
       <c r="G13" s="35">
         <f>SUMPRODUCT(F15:F22,G15:G22)/SUM(F15:F22)</f>
-        <v>0.84534883720930232</v>
+        <v>0.98255813953488369</v>
       </c>
       <c r="H13" s="29">
         <f t="shared" ref="H13:H17" si="0">NETWORKDAYS(D13,E13)</f>
@@ -4032,14 +4035,14 @@
       </c>
       <c r="I13" s="14">
         <f t="shared" ref="I13:I17" si="1">ROUNDDOWN(G13*F13,0)</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J13" s="29">
         <f>F13-I13</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="14" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A14" s="19"/>
       <c r="B14" s="50" t="s">
         <v>38</v>
@@ -4314,7 +4317,7 @@
       <c r="IP14" s="21"/>
       <c r="IQ14" s="21"/>
     </row>
-    <row r="15" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="15" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A15" s="19"/>
       <c r="B15" s="50" t="s">
         <v>41</v>
@@ -4589,7 +4592,7 @@
       <c r="IP15" s="21"/>
       <c r="IQ15" s="21"/>
     </row>
-    <row r="16" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="16" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A16" s="19"/>
       <c r="B16" s="50" t="s">
         <v>36</v>
@@ -4864,7 +4867,7 @@
       <c r="IP16" s="21"/>
       <c r="IQ16" s="21"/>
     </row>
-    <row r="17" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="17" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A17" s="19"/>
       <c r="B17" s="50" t="s">
         <v>35</v>
@@ -4883,7 +4886,7 @@
         <v>10</v>
       </c>
       <c r="G17" s="34">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H17" s="30">
         <f t="shared" si="0"/>
@@ -4891,11 +4894,11 @@
       </c>
       <c r="I17" s="12">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J17" s="30">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K17" s="21"/>
       <c r="L17" s="21"/>
@@ -5139,7 +5142,7 @@
       <c r="IP17" s="21"/>
       <c r="IQ17" s="21"/>
     </row>
-    <row r="18" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="18" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A18" s="19"/>
       <c r="B18" s="50" t="s">
         <v>22</v>
@@ -5158,7 +5161,7 @@
         <v>12</v>
       </c>
       <c r="G18" s="34">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="H18" s="30">
         <f>NETWORKDAYS(D18,E18)</f>
@@ -5166,11 +5169,11 @@
       </c>
       <c r="I18" s="12">
         <f>ROUNDDOWN(G18*F18,0)</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J18" s="30">
         <f>F18-I18</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
@@ -5414,7 +5417,7 @@
       <c r="IP18" s="21"/>
       <c r="IQ18" s="21"/>
     </row>
-    <row r="19" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="19" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A19" s="49"/>
       <c r="B19" s="50" t="s">
         <v>23</v>
@@ -5433,7 +5436,7 @@
         <v>10</v>
       </c>
       <c r="G19" s="34">
-        <v>0.35</v>
+        <v>0.85</v>
       </c>
       <c r="H19" s="30">
         <f t="shared" ref="H19:H23" si="13">NETWORKDAYS(D19,E19)</f>
@@ -5441,11 +5444,11 @@
       </c>
       <c r="I19" s="12">
         <f t="shared" ref="I19:I23" si="14">ROUNDDOWN(G19*F19,0)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J19" s="30">
         <f t="shared" ref="J19:J22" si="15">F19-I19</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
@@ -5689,13 +5692,13 @@
       <c r="IP19" s="21"/>
       <c r="IQ19" s="21"/>
     </row>
-    <row r="20" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="20" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A20" s="49"/>
       <c r="B20" s="50" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D20" s="36">
         <v>41036</v>
@@ -5964,7 +5967,7 @@
       <c r="IP20" s="21"/>
       <c r="IQ20" s="21"/>
     </row>
-    <row r="21" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="21" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A21" s="49"/>
       <c r="B21" s="50" t="s">
         <v>43</v>
@@ -6239,13 +6242,13 @@
       <c r="IP21" s="21"/>
       <c r="IQ21" s="21"/>
     </row>
-    <row r="22" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="22" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A22" s="49"/>
       <c r="B22" s="50" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D22" s="36">
         <v>41056</v>
@@ -6514,7 +6517,7 @@
       <c r="IP22" s="21"/>
       <c r="IQ22" s="21"/>
     </row>
-    <row r="23" spans="1:251" s="20" customFormat="1" ht="10">
+    <row r="23" spans="1:251" s="20" customFormat="1" ht="10.199999999999999">
       <c r="A23" s="47"/>
       <c r="B23" s="48" t="s">
         <v>24</v>
@@ -6533,7 +6536,7 @@
       </c>
       <c r="G23" s="35">
         <f>SUMPRODUCT(F24:F28,G24:G28)/SUM(F24:F28)</f>
-        <v>0.2986111111111111</v>
+        <v>0.62175925925925923</v>
       </c>
       <c r="H23" s="29">
         <f t="shared" si="13"/>
@@ -6541,20 +6544,20 @@
       </c>
       <c r="I23" s="14">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="J23" s="29">
         <f>F23-I23</f>
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="24" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A24" s="19"/>
       <c r="B24" s="50" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D24" s="36">
         <v>41054</v>
@@ -6567,7 +6570,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="34">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="H24" s="30">
         <f>NETWORKDAYS(D24,E24)</f>
@@ -6823,13 +6826,13 @@
       <c r="IP24" s="21"/>
       <c r="IQ24" s="21"/>
     </row>
-    <row r="25" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="25" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A25" s="19"/>
       <c r="B25" s="50" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D25" s="36">
         <v>41054</v>
@@ -6842,7 +6845,7 @@
         <v>25</v>
       </c>
       <c r="G25" s="34">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="H25" s="30">
         <f>NETWORKDAYS(D25,E25)</f>
@@ -6850,11 +6853,11 @@
       </c>
       <c r="I25" s="12">
         <f>ROUNDDOWN(G25*F25,0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J25" s="30">
         <f>F25-I25</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K25" s="21"/>
       <c r="L25" s="21"/>
@@ -7098,13 +7101,13 @@
       <c r="IP25" s="21"/>
       <c r="IQ25" s="21"/>
     </row>
-    <row r="26" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="26" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A26" s="19"/>
       <c r="B26" s="50" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D26" s="36">
         <v>41064</v>
@@ -7117,7 +7120,7 @@
         <v>26</v>
       </c>
       <c r="G26" s="34">
-        <v>0.6</v>
+        <v>0.85</v>
       </c>
       <c r="H26" s="30">
         <f t="shared" ref="H26" si="21">NETWORKDAYS(D26,E26)</f>
@@ -7125,11 +7128,11 @@
       </c>
       <c r="I26" s="12">
         <f t="shared" ref="I26" si="22">ROUNDDOWN(G26*F26,0)</f>
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="J26" s="30">
         <f t="shared" ref="J26" si="23">F26-I26</f>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="K26" s="21"/>
       <c r="L26" s="21"/>
@@ -7373,13 +7376,13 @@
       <c r="IP26" s="21"/>
       <c r="IQ26" s="21"/>
     </row>
-    <row r="27" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="27" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A27" s="49"/>
       <c r="B27" s="50" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D27" s="36">
         <v>41070</v>
@@ -7648,13 +7651,13 @@
       <c r="IP27" s="21"/>
       <c r="IQ27" s="21"/>
     </row>
-    <row r="28" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="28" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A28" s="49"/>
       <c r="B28" s="50" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D28" s="36">
         <v>41054</v>
@@ -7667,7 +7670,7 @@
         <v>36</v>
       </c>
       <c r="G28" s="34">
-        <v>0.1</v>
+        <v>0.85</v>
       </c>
       <c r="H28" s="30">
         <f>NETWORKDAYS(D28,E28)</f>
@@ -7675,11 +7678,11 @@
       </c>
       <c r="I28" s="12">
         <f>ROUNDDOWN(G28*F28,0)</f>
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="J28" s="30">
         <f>F28-I28</f>
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
@@ -7923,7 +7926,7 @@
       <c r="IP28" s="21"/>
       <c r="IQ28" s="21"/>
     </row>
-    <row r="29" spans="1:251" s="20" customFormat="1" ht="10">
+    <row r="29" spans="1:251" s="20" customFormat="1" ht="10.199999999999999">
       <c r="A29" s="47"/>
       <c r="B29" s="48" t="s">
         <v>28</v>
@@ -7957,13 +7960,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="30" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A30" s="19"/>
       <c r="B30" s="50" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D30" s="36">
         <v>41069</v>
@@ -8232,7 +8235,7 @@
       <c r="IP30" s="21"/>
       <c r="IQ30" s="21"/>
     </row>
-    <row r="31" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="31" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A31" s="19"/>
       <c r="B31" s="50" t="s">
         <v>31</v>
@@ -8507,7 +8510,7 @@
       <c r="IP31" s="21"/>
       <c r="IQ31" s="21"/>
     </row>
-    <row r="32" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="32" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A32" s="49"/>
       <c r="B32" s="50" t="s">
         <v>32</v>
@@ -8782,7 +8785,7 @@
       <c r="IP32" s="21"/>
       <c r="IQ32" s="21"/>
     </row>
-    <row r="33" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="33" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A33" s="49"/>
       <c r="B33" s="50" t="s">
         <v>42</v>
@@ -9057,7 +9060,7 @@
       <c r="IP33" s="21"/>
       <c r="IQ33" s="21"/>
     </row>
-    <row r="34" spans="1:251" s="20" customFormat="1" ht="10">
+    <row r="34" spans="1:251" s="20" customFormat="1" ht="10.199999999999999">
       <c r="A34" s="47"/>
       <c r="B34" s="48" t="s">
         <v>33</v>
@@ -9091,7 +9094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:251" s="23" customFormat="1" ht="10">
+    <row r="35" spans="1:251" s="23" customFormat="1" ht="10.199999999999999">
       <c r="A35" s="19"/>
       <c r="B35" s="50" t="s">
         <v>19</v>
@@ -9368,38 +9371,6 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="HD11:HH11"/>
-    <mergeCell ref="HI11:HM11"/>
-    <mergeCell ref="HN11:HR11"/>
-    <mergeCell ref="HS11:HW11"/>
-    <mergeCell ref="GJ11:GN11"/>
-    <mergeCell ref="GO11:GS11"/>
-    <mergeCell ref="GT11:GX11"/>
-    <mergeCell ref="GY11:HC11"/>
-    <mergeCell ref="FP11:FT11"/>
-    <mergeCell ref="FU11:FY11"/>
-    <mergeCell ref="FZ11:GD11"/>
-    <mergeCell ref="GE11:GI11"/>
-    <mergeCell ref="EV11:EZ11"/>
-    <mergeCell ref="FA11:FE11"/>
-    <mergeCell ref="FF11:FJ11"/>
-    <mergeCell ref="FK11:FO11"/>
-    <mergeCell ref="EB11:EF11"/>
-    <mergeCell ref="EG11:EK11"/>
-    <mergeCell ref="EL11:EP11"/>
-    <mergeCell ref="EQ11:EU11"/>
-    <mergeCell ref="DH11:DL11"/>
-    <mergeCell ref="DM11:DQ11"/>
-    <mergeCell ref="DR11:DV11"/>
-    <mergeCell ref="DW11:EA11"/>
-    <mergeCell ref="CN11:CR11"/>
-    <mergeCell ref="CS11:CW11"/>
-    <mergeCell ref="CX11:DB11"/>
-    <mergeCell ref="DC11:DG11"/>
-    <mergeCell ref="BT11:BX11"/>
-    <mergeCell ref="BY11:CC11"/>
-    <mergeCell ref="CD11:CH11"/>
-    <mergeCell ref="CI11:CM11"/>
     <mergeCell ref="IH11:IL11"/>
     <mergeCell ref="IM11:IQ11"/>
     <mergeCell ref="L11:P11"/>
@@ -9416,6 +9387,38 @@
     <mergeCell ref="AK11:AO11"/>
     <mergeCell ref="AP11:AT11"/>
     <mergeCell ref="AU11:AY11"/>
+    <mergeCell ref="CN11:CR11"/>
+    <mergeCell ref="CS11:CW11"/>
+    <mergeCell ref="CX11:DB11"/>
+    <mergeCell ref="DC11:DG11"/>
+    <mergeCell ref="BT11:BX11"/>
+    <mergeCell ref="BY11:CC11"/>
+    <mergeCell ref="CD11:CH11"/>
+    <mergeCell ref="CI11:CM11"/>
+    <mergeCell ref="EB11:EF11"/>
+    <mergeCell ref="EG11:EK11"/>
+    <mergeCell ref="EL11:EP11"/>
+    <mergeCell ref="EQ11:EU11"/>
+    <mergeCell ref="DH11:DL11"/>
+    <mergeCell ref="DM11:DQ11"/>
+    <mergeCell ref="DR11:DV11"/>
+    <mergeCell ref="DW11:EA11"/>
+    <mergeCell ref="FP11:FT11"/>
+    <mergeCell ref="FU11:FY11"/>
+    <mergeCell ref="FZ11:GD11"/>
+    <mergeCell ref="GE11:GI11"/>
+    <mergeCell ref="EV11:EZ11"/>
+    <mergeCell ref="FA11:FE11"/>
+    <mergeCell ref="FF11:FJ11"/>
+    <mergeCell ref="FK11:FO11"/>
+    <mergeCell ref="HD11:HH11"/>
+    <mergeCell ref="HI11:HM11"/>
+    <mergeCell ref="HN11:HR11"/>
+    <mergeCell ref="HS11:HW11"/>
+    <mergeCell ref="GJ11:GN11"/>
+    <mergeCell ref="GO11:GS11"/>
+    <mergeCell ref="GT11:GX11"/>
+    <mergeCell ref="GY11:HC11"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="L13:IQ13 L30:IQ30 L24:IQ24 L35:IQ35">
@@ -9458,7 +9461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -9466,7 +9469,7 @@
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>